<commit_message>
Now replaces inf values in yield corrected maps with zero.
</commit_message>
<xml_diff>
--- a/mineral_library.xlsx
+++ b/mineral_library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\CoSE\SNS\CODES\ICPMSLab\R&amp;D\Ivan\250523_A_TOF_MeltEmbayments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\CoSE\SNS\CODES\ICPMSLab\Software\Jeff's Python Backups\CODES-LazAbMapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB62B61E-77B0-4C80-A215-EE28BE7A2DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC38F46C-AFEC-43E6-AEDA-70960B4B2F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13780" yWindow="2850" windowWidth="23020" windowHeight="13320" xr2:uid="{97E58254-DB34-406F-B147-6544DE51B774}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{97E58254-DB34-406F-B147-6544DE51B774}"/>
   </bookViews>
   <sheets>
     <sheet name="silicates" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="128">
   <si>
     <t>mineral name</t>
   </si>
@@ -448,6 +448,9 @@
   </si>
   <si>
     <t>epoxy</t>
+  </si>
+  <si>
+    <t>scheelite</t>
   </si>
 </sst>
 </file>
@@ -1344,22 +1347,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491FE880-6296-4FFD-9FC5-5C2168F3E915}">
-  <dimension ref="A1:CB44"/>
+  <dimension ref="A1:CB45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="BO38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="BJ20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CA48" sqref="CA48"/>
+      <selection pane="bottomRight" activeCell="BO45" sqref="BO45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7265625" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1601,7 +1604,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1672,7 +1675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1743,7 +1746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1814,7 +1817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1885,7 +1888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1956,7 +1959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -2027,7 +2030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2098,7 +2101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2169,7 +2172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2240,7 +2243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2302,7 +2305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2373,7 +2376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -2444,7 +2447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2515,7 +2518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -2586,7 +2589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -2654,7 +2657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2725,7 +2728,7 @@
         <v>1.0415722120658135</v>
       </c>
     </row>
-    <row r="18" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -2750,7 +2753,7 @@
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
     </row>
-    <row r="19" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -2785,7 +2788,7 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="20" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -2808,7 +2811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -2840,7 +2843,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="22" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -2881,7 +2884,7 @@
         <v>8.7200000000000006</v>
       </c>
     </row>
-    <row r="23" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -2913,7 +2916,7 @@
         <v>22.52</v>
       </c>
     </row>
-    <row r="24" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -2945,7 +2948,7 @@
         <v>19.52</v>
       </c>
     </row>
-    <row r="25" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -2980,7 +2983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -3009,7 +3012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -3029,7 +3032,7 @@
         <v>4.6900000000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>108</v>
       </c>
@@ -3055,7 +3058,7 @@
         <v>48.72</v>
       </c>
     </row>
-    <row r="29" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>109</v>
       </c>
@@ -3177,7 +3180,7 @@
         <v>1.274204924519046E-5</v>
       </c>
     </row>
-    <row r="30" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>111</v>
       </c>
@@ -3212,7 +3215,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="31" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>112</v>
       </c>
@@ -3337,7 +3340,7 @@
         <v>3.2740755555555554E-6</v>
       </c>
     </row>
-    <row r="32" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>113</v>
       </c>
@@ -3363,7 +3366,7 @@
         <v>35.03</v>
       </c>
     </row>
-    <row r="33" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>114</v>
       </c>
@@ -3488,7 +3491,7 @@
         <v>9.4883537563903882E-6</v>
       </c>
     </row>
-    <row r="34" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>115</v>
       </c>
@@ -3541,7 +3544,7 @@
         <v>2.1666666666666667E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>116</v>
       </c>
@@ -3573,7 +3576,7 @@
         <v>18.16</v>
       </c>
     </row>
-    <row r="36" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>117</v>
       </c>
@@ -3602,7 +3605,7 @@
         <v>86.5</v>
       </c>
     </row>
-    <row r="37" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>118</v>
       </c>
@@ -3622,7 +3625,7 @@
         <v>60.18</v>
       </c>
     </row>
-    <row r="38" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>119</v>
       </c>
@@ -3651,7 +3654,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>120</v>
       </c>
@@ -3680,7 +3683,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="40" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>121</v>
       </c>
@@ -3805,7 +3808,7 @@
         <v>4.6645134243034008E-6</v>
       </c>
     </row>
-    <row r="41" spans="1:80" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:80" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>122</v>
       </c>
@@ -3822,7 +3825,7 @@
         <v>59.94</v>
       </c>
     </row>
-    <row r="42" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>124</v>
       </c>
@@ -3842,7 +3845,7 @@
         <v>29.44</v>
       </c>
     </row>
-    <row r="43" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>125</v>
       </c>
@@ -3865,10 +3868,13 @@
         <v>14.57</v>
       </c>
     </row>
-    <row r="44" spans="1:80" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>126</v>
       </c>
+      <c r="C44">
+        <v>43</v>
+      </c>
       <c r="D44">
         <v>0</v>
       </c>
@@ -4099,6 +4105,26 @@
       </c>
       <c r="CB44">
         <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>127</v>
+      </c>
+      <c r="B45" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45">
+        <v>44</v>
+      </c>
+      <c r="L45">
+        <v>13.92</v>
+      </c>
+      <c r="M45">
+        <v>13.92</v>
+      </c>
+      <c r="BO45">
+        <v>63.85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>